<commit_message>
changed colname of RT
</commit_message>
<xml_diff>
--- a/shiny_app/KI_upload_template.xlsx
+++ b/shiny_app/KI_upload_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruy/Documents/Github_R/KI_calculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruy/Documents/Github_R/KI_calculator/shiny_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4412E7B6-CB81-7940-906B-D04B92AD5EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3800A3-A10E-8846-A49C-DC74AA036E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="1040" windowWidth="27640" windowHeight="15480" activeTab="1" xr2:uid="{39BFF476-E97E-8F46-A494-108C04796D1A}"/>
+    <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15480" activeTab="1" xr2:uid="{39BFF476-E97E-8F46-A494-108C04796D1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Alkane_Series" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>carbons</t>
   </si>
   <si>
-    <t>RT_seconds</t>
-  </si>
-  <si>
     <t>n-octane</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>unknown_5</t>
+  </si>
+  <si>
+    <t>retention_time</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A63FAF-9D7A-164E-8175-A6FB0FC5FCCB}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -473,12 +475,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -489,7 +491,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -500,7 +502,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -511,7 +513,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -522,7 +524,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -533,7 +535,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>13</v>
@@ -544,7 +546,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -555,7 +557,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -566,7 +568,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -577,7 +579,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>17</v>
@@ -588,7 +590,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>18</v>
@@ -599,7 +601,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>19</v>
@@ -617,7 +619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058F3AD5-49CD-0942-8A3F-ED8FDED8916B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -626,15 +630,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>906.8</v>
@@ -642,7 +646,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>1021.4</v>
@@ -650,7 +654,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>1300</v>
@@ -658,7 +662,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>1506.6</v>
@@ -666,7 +670,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>1000.1</v>

</xml_diff>

<commit_message>
changed example comound IDs
</commit_message>
<xml_diff>
--- a/shiny_app/KI_upload_template.xlsx
+++ b/shiny_app/KI_upload_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruy/Documents/Github_R/KI_calculator/shiny_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3800A3-A10E-8846-A49C-DC74AA036E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772843F9-BB0A-264A-BD0E-4473040201AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15480" activeTab="1" xr2:uid="{39BFF476-E97E-8F46-A494-108C04796D1A}"/>
   </bookViews>
@@ -83,22 +83,22 @@
     <t>compound_id</t>
   </si>
   <si>
-    <t>unknown_1</t>
-  </si>
-  <si>
-    <t>unknown_2</t>
-  </si>
-  <si>
-    <t>unknown_3</t>
-  </si>
-  <si>
-    <t>unknown_4</t>
-  </si>
-  <si>
-    <t>unknown_5</t>
-  </si>
-  <si>
     <t>retention_time</t>
+  </si>
+  <si>
+    <t>my_compound_1</t>
+  </si>
+  <si>
+    <t>my_compound_2</t>
+  </si>
+  <si>
+    <t>my_compound_3</t>
+  </si>
+  <si>
+    <t>my_compound_4</t>
+  </si>
+  <si>
+    <t>my_compound_5</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -620,7 +620,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,12 +633,12 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>906.8</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1021.4</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1300</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>1506.6</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>1000.1</v>

</xml_diff>